<commit_message>
arrange checkout page and comments for save details and sort products
</commit_message>
<xml_diff>
--- a/viasus/report.xlsx
+++ b/viasus/report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,46 +441,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0010003000079</t>
+          <t xml:space="preserve">0010017000044       </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MANZANAS ALUMINIO MHB04 36H RS D TUERCA STL MORADO</t>
+          <t xml:space="preserve">ABRAZADERA MARCO SILLA POLISPORT                  </t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0010003000008       </t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PASTILLAS FRENOS ACERO MDA01 STL. HPD02-PAR       </t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0010003000018       </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">FRENOS VBRAKE ALUMINIO TWISTER HVK140 NEGRO - SET </t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>